<commit_message>
reportes en excel adelantado
</commit_message>
<xml_diff>
--- a/reportePRuebas.xlsx
+++ b/reportePRuebas.xlsx
@@ -7,9 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PRUEBA" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="HojaPrueba" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="HojaPrueba2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Reporte Prueba" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -48,8 +46,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -415,50 +416,348 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>RESULTADO DE GOOGLE VISION</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>NOMBRE DE LA IMAGEN</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>RUTA DE LA IMAGEN</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">33
+Anest
+Beatos
+SOS
+Pes
+Uhiese
+Coradin
+3012218
+De
+he's
+SAN BENEDETTO
+IMPORTACHI
+RAZ
+Contend
+Akerst
+NATURAL MINERAL WATER
+Cont. Net. 500ml
+Shes P
+Set 38
+2013
+Corse
+STILL
+</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Agua0.JPG</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>C:\Users\Joan Colina\Desktop\miCosas\Semestre9\PDG\proyectoClonado\IsoaparienciasPDG\Images\Agua\Agua0.JPG</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bebida Mista de Uva,
+Maçã e Limão
+Agite Antes de Beber
+Bebida Mb
+Diabetios com
+água mineral
+maça lime
+benzoato de su
+potássio Nu
+santana (N-50
+i), sequestra
+(INS-385acali
+aroma natura
+S. (INS-123e
+Não alcoolice
+vide marcar
+gara. Na
+Produits
+Alimentos
+loci Fenster
+Campos do
+0002-22
+Citrus
+no SPATE
+COM
+en avomatteante e sucos naturais Conteudo 250ml
+7189616
+</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>Agua1.JPG</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>C:\Users\Joan Colina\Desktop\miCosas\Semestre9\PDG\proyectoClonado\IsoaparienciasPDG\Images\Agua\Agua1.JPG</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">23
+50
+Naranjada
+Refrescante
+Naturalmente
+con vitamina C
+</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Agua2.JPG</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>C:\Users\Joan Colina\Desktop\miCosas\Semestre9\PDG\proyectoClonado\IsoaparienciasPDG\Images\Agua\Agua2.JPG</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">600 mL,
+eno
+Agua
+Potable
+Tratada
+Agua 100%
+Lalala
+Oy
+Ver
+</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>Agua3.JPG</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>C:\Users\Joan Colina\Desktop\miCosas\Semestre9\PDG\proyectoClonado\IsoaparienciasPDG\Images\Agua\Agua3.JPG</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">be
+OLUN
+AGUA MINERAL NATURAL
+ENVASADO POR: MAGRILLANO SAS
+EN SU ORIGEN
+VEREDA EL CARMEN, VILLAVICENCIO, META
+Desde 1985
+Реdіdоs:(1) 250 2332
+Bogotá
+SAR
+(
+ОТИТЕ
+1
+DET
+390 AUDA
+LIBRERIA
+NACIONAL
+</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>Agua4.JPG</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>C:\Users\Joan Colina\Desktop\miCosas\Semestre9\PDG\proyectoClonado\IsoaparienciasPDG\Images\Agua\Agua4.JPG</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">23
+TRATTORIN
+CIN A
+ITALIAN
+WWW.LATRATTORINA.COM
+</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>Agua5.JPG</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>C:\Users\Joan Colina\Desktop\miCosas\Semestre9\PDG\proyectoClonado\IsoaparienciasPDG\Images\Agua\Agua5.JPG</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">&gt;
+13
+Doña
+Francia
+Agua Mineral Natural
+500 ml.
+</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>Agua6.JPG</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>C:\Users\Joan Colina\Desktop\miCosas\Semestre9\PDG\proyectoClonado\IsoaparienciasPDG\Images\Agua\Agua6.JPG</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1104
+87
+NATURAL DE MANANTIAL
+ettes de niebla
+a mortales del
+Caca, en la
+a les Munopio de
+asa de Buga
+lagroso Brola pura,
+sajosalina
+red de Manantial
+CLINICA
+INTERPLASTICA
+alia
+GRUPO INTERNACIONAL
+DE ESPECIALISTAS
+EN CIRUGIA PLASTICA
+al praua sa s
+a dua an sa s
+wait Cale 5#1-28
+2012-317 6610268
+385-3173010919
+asas@hotmail.com
+rate Buga
+aca-Colombia
+wao SAV191 14610
+Colombiana
+en el menos
+mente antes de
+GEMISE
+Calle 5C Nº 43 - 10 Cali
+PBX: 5532407
+3155694208
+www.clinicainterplasticacali.com
+</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>Agua7.JPG</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>C:\Users\Joan Colina\Desktop\miCosas\Semestre9\PDG\proyectoClonado\IsoaparienciasPDG\Images\Agua\Agua7.JPG</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">32
+de
+Cont. Neto
+250 ml
+LAN
+El encanto de volar
+GRUPO LATAM AIRLINES
+</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>Agua8.JPG</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>C:\Users\Joan Colina\Desktop\miCosas\Semestre9\PDG\proyectoClonado\IsoaparienciasPDG\Images\Agua\Agua8.JPG</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">*
+vel
+agua con colágeno
+pepino y limón
+635 ml / 21 oz
+Bebida de agua con colágeno
+y extracto de pepino sabor a limon
+33
+33
+32
+33
+L0402164
+VO3AG016
+</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>Agua9.JPG</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>C:\Users\Joan Colina\Desktop\miCosas\Semestre9\PDG\proyectoClonado\IsoaparienciasPDG\Images\Agua\Agua9.JPG</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>